<commit_message>
Run income classifiers, retrieve model results, and produce graphs
</commit_message>
<xml_diff>
--- a/Model Comparison.xlsx
+++ b/Model Comparison.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17085" windowHeight="2415" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="2040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wine Dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="Titanic Dataset" sheetId="2" r:id="rId2"/>
+    <sheet name="Income Dataset" sheetId="3" r:id="rId2"/>
+    <sheet name="Titanic Dataset" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t>Model</t>
   </si>
@@ -115,6 +116,18 @@
   </si>
   <si>
     <t>learning rate: 0.005</t>
+  </si>
+  <si>
+    <t>kernel: linear</t>
+  </si>
+  <si>
+    <t>number of neighbors: 10</t>
+  </si>
+  <si>
+    <t>hidden layer size: 3</t>
+  </si>
+  <si>
+    <t>learning rate: 0.01</t>
   </si>
 </sst>
 </file>
@@ -489,7 +502,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,8 +677,193 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="H2" s="2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.86829999999999996</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.83540000000000003</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2916</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="H5" s="2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>